<commit_message>
Reverted change "room for arrow"
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/AddingDataSet.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/AddingDataSet.xlsx
@@ -465,10 +465,10 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="16.175425" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="14.145425" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="16.195425" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="14.015425" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="12.175425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.150625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="12.195425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="11.330625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4">
@@ -577,10 +577,10 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="16.175425" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="14.145425" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="16.195425" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="14.015425" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="12.175425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.150625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="12.195425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="11.330625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4">
@@ -689,10 +689,10 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="16.175425" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="14.145425" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="16.195425" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="14.015425" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="12.175425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.150625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="12.195425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="11.330625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4">

</xml_diff>

<commit_message>
Add ability to set table name when adding a worksheet with datatable - Fixes Issue #1712
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/AddingDataSet.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/AddingDataSet.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Patients" displayName="Patients" ref="A1:D6" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0">
   <x:autoFilter ref="A1:D6"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="Dosage"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Employees" displayName="Employees" ref="A1:D6" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D6" totalsRowShown="0">
   <x:autoFilter ref="A1:D6"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="Dosage"/>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Information" displayName="Information" ref="A1:D6" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D6" totalsRowShown="0">
   <x:autoFilter ref="A1:D6"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="Dosage"/>

</xml_diff>